<commit_message>
Fixed price and added historical function
</commit_message>
<xml_diff>
--- a/api Manager/report_config.xlsx
+++ b/api Manager/report_config.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torem\Dropbox\RLC Documents\LLM Model and Documents\Projects\api Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE1EF4E-5BEA-4333-B7E0-661136C87AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D1E156-A22F-452C-8250-41BB4DE471B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{ADF9F7D8-176C-4D97-B2A6-BAFF23809C54}"/>
+    <workbookView xWindow="-27240" yWindow="1560" windowWidth="24450" windowHeight="13785" xr2:uid="{ADF9F7D8-176C-4D97-B2A6-BAFF23809C54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Inactive" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="117">
   <si>
     <t>id</t>
   </si>
@@ -190,13 +193,283 @@
   </si>
   <si>
     <t xml:space="preserve">Weekly corn stalks, straw, and grass </t>
+  </si>
+  <si>
+    <t>OKC West Livestock Auction – El Reno, OK</t>
+  </si>
+  <si>
+    <t>cattle</t>
+  </si>
+  <si>
+    <t>AMS_1281</t>
+  </si>
+  <si>
+    <t>Weekly feeder cattle auction prices (Medium &amp; Large #1 steers, 450–800 lb)</t>
+  </si>
+  <si>
+    <t>livestock</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/1281</t>
+  </si>
+  <si>
+    <t>National Weekly Direct Slaughter Cattle – Negotiated Purchases</t>
+  </si>
+  <si>
+    <t>AMS_2477</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/2477</t>
+  </si>
+  <si>
+    <t>Nebraska Weekly Direct Slaughter Cattle – Negotiated Purchases</t>
+  </si>
+  <si>
+    <t>AMS_2485</t>
+  </si>
+  <si>
+    <t>Weekly Nebraska direct slaughter cattle negotiated cash prices</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/2485</t>
+  </si>
+  <si>
+    <t>Cattle Country Livestock Video/Internet Auction – Torrington, WY</t>
+  </si>
+  <si>
+    <t>AMS_2675</t>
+  </si>
+  <si>
+    <t>Feeder cattle prices from video/internet auction (Torrington, WY)</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/2675</t>
+  </si>
+  <si>
+    <t>poultry</t>
+  </si>
+  <si>
+    <t>AMS_2771</t>
+  </si>
+  <si>
+    <t>Daily summary of national turkey market prices and conditions</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/2771</t>
+  </si>
+  <si>
+    <t>swine</t>
+  </si>
+  <si>
+    <t>AMS_2810</t>
+  </si>
+  <si>
+    <t>Weekly feeder pig prices (early-weaned 10–12 lb and 40 lb pigs)</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/2810</t>
+  </si>
+  <si>
+    <t>National Daily Sunflower, Canola, Millet, and Flaxseed Report</t>
+  </si>
+  <si>
+    <t>AMS_2887</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/2887</t>
+  </si>
+  <si>
+    <t>Indiana Grain Bids</t>
+  </si>
+  <si>
+    <t>AMS_2932</t>
+  </si>
+  <si>
+    <t>Daily grain elevator bid prices in Indiana (corn, soybeans, etc.)</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/2932</t>
+  </si>
+  <si>
+    <t>Green City Livestock Auction – Green City, MO</t>
+  </si>
+  <si>
+    <t>AMS_3046</t>
+  </si>
+  <si>
+    <t>Feeder cattle auction prices (Missouri)</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/3046</t>
+  </si>
+  <si>
+    <t>AMS_3148</t>
+  </si>
+  <si>
+    <t>Daily wheat bid prices – Kansas City market (HRW wheat)</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/3148</t>
+  </si>
+  <si>
+    <t>Illinois Grain Bids</t>
+  </si>
+  <si>
+    <t>AMS_3192</t>
+  </si>
+  <si>
+    <t>Daily grain elevator bid prices in Illinois (corn, soybeans, etc.)</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/3192</t>
+  </si>
+  <si>
+    <t>Illinois Production Cost Report (Bi-Weekly)</t>
+  </si>
+  <si>
+    <t>AMS_3195</t>
+  </si>
+  <si>
+    <t>Bi-weekly prices of farm input costs in Illinois (fuel &amp; fertilizer)</t>
+  </si>
+  <si>
+    <t>bi-weekly</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/3195</t>
+  </si>
+  <si>
+    <t>Ohio Daily Grain Bids</t>
+  </si>
+  <si>
+    <t>AMS_3225</t>
+  </si>
+  <si>
+    <t>Daily grain elevator bid prices in Ohio (corn, soybeans, etc.)</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/3225</t>
+  </si>
+  <si>
+    <t>AMS_3511</t>
+  </si>
+  <si>
+    <t>Weekly prices for grain by-product feedstuffs (e.g. soybean meal, millfeeds)</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/3511</t>
+  </si>
+  <si>
+    <t>Weekly Cotton Market Review (CNWWCMR)</t>
+  </si>
+  <si>
+    <t>cotton</t>
+  </si>
+  <si>
+    <t>CNWWCMR</t>
+  </si>
+  <si>
+    <t>Weekly cotton spot market review and price summary (Upland cotton)</t>
+  </si>
+  <si>
+    <t>https://mymarketnews.ams.usda.gov/viewReport/3024</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Weekly </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5-Area direct slaughter cattle cash prices (negotiated trade)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Turkey:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Daily National Turkey Market-at-a-Glance</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">National Direct </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Feeder Pig Report</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Daily cash prices for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sunflower, canola, millet, and flaxseed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kansas City Board of Trade </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Daily Wheat Bids</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">National Grain and Oilseed Processor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Feedstuff Report</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,13 +504,40 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF18453B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBEAD2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -253,12 +553,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -266,6 +570,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF18453B"/>
+      <color rgb="FFDBEAD2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -275,6 +585,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Formulas"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Text"/>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -594,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEA98E3F-259D-4B7E-832B-A9BEDD9DE859}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A23" sqref="A23:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,31 +946,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -814,6 +1146,522 @@
       </c>
       <c r="I7" s="3" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>1281</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2477</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2485</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2675</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2771</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2810</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>2887</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>2932</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>3046</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>3148</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>3192</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>3195</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>3225</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>3511</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>3024</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f>RIGHT([1]Sheet2!$W56,4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <f>RIGHT([1]Sheet2!$W57,4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f>RIGHT([1]Sheet2!$W58,4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
+        <f>RIGHT([1]Sheet2!$W59,4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
+        <f>RIGHT([1]Sheet2!$W60,4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
+        <f>RIGHT([1]Sheet2!$W61,4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="str">
+        <f>RIGHT([1]Sheet2!$W62,4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="str">
+        <f>RIGHT([1]Sheet2!$W63,4)</f>
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -821,6 +1669,21 @@
     <hyperlink ref="I5" r:id="rId1" xr:uid="{1654460B-225E-4700-AC8D-A65B57357A67}"/>
     <hyperlink ref="I6" r:id="rId2" xr:uid="{C13F3259-A522-4F3D-90DE-8776328594D6}"/>
     <hyperlink ref="I7" r:id="rId3" xr:uid="{45FE8ECC-5864-4A52-BCF5-FDFA002DFE35}"/>
+    <hyperlink ref="I8" r:id="rId4" xr:uid="{B74A878D-57F8-49E2-A2C6-901064E8B39C}"/>
+    <hyperlink ref="I9" r:id="rId5" xr:uid="{8F074E40-B35F-4DC9-8A35-29FC448E060A}"/>
+    <hyperlink ref="I10" r:id="rId6" xr:uid="{078A2F78-C1C4-4B30-909B-672336E38453}"/>
+    <hyperlink ref="I11" r:id="rId7" xr:uid="{CA510728-0937-4EF3-9FCB-2F08CC7DEC03}"/>
+    <hyperlink ref="I12" r:id="rId8" xr:uid="{DE673F28-97B7-437A-BAB6-7EBF2CDA3CB1}"/>
+    <hyperlink ref="I13" r:id="rId9" xr:uid="{42F75FE9-EEE4-4F5C-835B-29588F1BD65E}"/>
+    <hyperlink ref="I14" r:id="rId10" xr:uid="{25E27830-9D9A-45DA-A360-DA7DFC7A4640}"/>
+    <hyperlink ref="I15" r:id="rId11" xr:uid="{F4B31312-DE0E-4651-A8D4-F733894998DD}"/>
+    <hyperlink ref="I16" r:id="rId12" xr:uid="{573FF64B-CED2-4C32-BD9C-7B4DE7EA6191}"/>
+    <hyperlink ref="I17" r:id="rId13" xr:uid="{D1AB433A-0410-4787-B451-1EF384FA1AA5}"/>
+    <hyperlink ref="I18" r:id="rId14" xr:uid="{BC4B2502-DF29-4685-9737-BF753CE72C2B}"/>
+    <hyperlink ref="I19" r:id="rId15" xr:uid="{8925C758-2D6A-455F-829D-62F4243D4A18}"/>
+    <hyperlink ref="I20" r:id="rId16" xr:uid="{57A326E2-8800-4220-9A3E-9C887EAAC93F}"/>
+    <hyperlink ref="I21" r:id="rId17" xr:uid="{BB91C4DD-5DA6-4D15-9395-8DDF804CBA95}"/>
+    <hyperlink ref="I22" r:id="rId18" xr:uid="{52A077D0-EEAE-40F0-9197-23A759312FF4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>